<commit_message>
Criando o Loop e o tempo de atualização  para vários cadastros
</commit_message>
<xml_diff>
--- a/Filiais.xlsx
+++ b/Filiais.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7e32da25853bd735/Área de Trabalho/Nova pasta/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D703FF8E-40FC-4AD2-AB23-06D77A001340}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="67" documentId="8_{D703FF8E-40FC-4AD2-AB23-06D77A001340}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2099045E-5CF4-4028-B5D6-57A67B7B1519}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{42B77C7D-5F13-4598-8FBB-EE9C3E20BED4}"/>
   </bookViews>
@@ -36,54 +36,51 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
-  <si>
-    <t>13765-Múltipla-24 de Outubro</t>
-  </si>
-  <si>
-    <t>18870-Múltipla-Av. Rio Verde</t>
-  </si>
-  <si>
-    <t>20022-Múltipla-Caldas Novas</t>
-  </si>
-  <si>
-    <t>21302-Múltipla-ER Garavelo</t>
-  </si>
-  <si>
-    <t>21546-Múltipla-ER Hidrolândia</t>
-  </si>
-  <si>
-    <t>21344-Múltipla-Senador Canedo</t>
-  </si>
-  <si>
-    <t>21825-Múltipla-Morada do Sol</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Nome da Filial</t>
   </si>
   <si>
-    <t>15.078.337/0001-99</t>
-  </si>
-  <si>
-    <t>15.078.337/0002-70</t>
-  </si>
-  <si>
-    <t>15.078.337/0003-50</t>
-  </si>
-  <si>
-    <t>15.078.337/0005-12</t>
-  </si>
-  <si>
-    <t>15.078.337/0006-01</t>
-  </si>
-  <si>
-    <t>15.078.337/0007-84</t>
+    <t>CNPJ</t>
+  </si>
+  <si>
+    <t>Fantasia</t>
   </si>
   <si>
     <t>15.078.337/0009-46</t>
   </si>
   <si>
-    <t>CNPJ</t>
+    <t>15.078.337/0004-31</t>
+  </si>
+  <si>
+    <t>20966-Multipla-Av. Mangalô</t>
+  </si>
+  <si>
+    <t>22001-Natureza-Av. Irany Trindade</t>
+  </si>
+  <si>
+    <t>02.870.566/0048-63</t>
+  </si>
+  <si>
+    <t>22011-Natureza-J. Rodrigues Goianira</t>
+  </si>
+  <si>
+    <t>02.870.566/0003-61</t>
+  </si>
+  <si>
+    <t>21825-Multipla-Morada do Sol</t>
+  </si>
+  <si>
+    <t>21825-Multipla</t>
+  </si>
+  <si>
+    <t>20966-Multipla</t>
+  </si>
+  <si>
+    <t>22001-Natureza</t>
+  </si>
+  <si>
+    <t>22011-Natureza</t>
   </si>
 </sst>
 </file>
@@ -136,6 +133,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -435,78 +436,71 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D0D9622-31EC-4FD3-8FA2-68D1F2266F0C}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>7</v>
       </c>
-      <c r="B1" t="s">
-        <v>15</v>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" t="s">
+      <c r="C5" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Corrgindo possiveis erros com Try exeption
</commit_message>
<xml_diff>
--- a/Filiais.xlsx
+++ b/Filiais.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7e32da25853bd735/Área de Trabalho/Nova pasta/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="67" documentId="8_{D703FF8E-40FC-4AD2-AB23-06D77A001340}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2099045E-5CF4-4028-B5D6-57A67B7B1519}"/>
+  <xr:revisionPtr revIDLastSave="120" documentId="8_{D703FF8E-40FC-4AD2-AB23-06D77A001340}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{40E26D7A-0664-4141-9625-138EEB958FB4}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{42B77C7D-5F13-4598-8FBB-EE9C3E20BED4}"/>
+    <workbookView xWindow="-24120" yWindow="1575" windowWidth="24240" windowHeight="13020" xr2:uid="{42B77C7D-5F13-4598-8FBB-EE9C3E20BED4}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
   <si>
     <t>Nome da Filial</t>
   </si>
@@ -47,48 +47,32 @@
     <t>Fantasia</t>
   </si>
   <si>
-    <t>15.078.337/0009-46</t>
-  </si>
-  <si>
-    <t>15.078.337/0004-31</t>
-  </si>
-  <si>
-    <t>20966-Multipla-Av. Mangalô</t>
-  </si>
-  <si>
-    <t>22001-Natureza-Av. Irany Trindade</t>
-  </si>
-  <si>
-    <t>02.870.566/0048-63</t>
-  </si>
-  <si>
-    <t>22011-Natureza-J. Rodrigues Goianira</t>
-  </si>
-  <si>
-    <t>02.870.566/0003-61</t>
-  </si>
-  <si>
-    <t>21825-Multipla-Morada do Sol</t>
-  </si>
-  <si>
-    <t>21825-Multipla</t>
-  </si>
-  <si>
-    <t>20966-Multipla</t>
-  </si>
-  <si>
-    <t>22001-Natureza</t>
-  </si>
-  <si>
-    <t>22011-Natureza</t>
+    <t>88.543.679/0001-06</t>
+  </si>
+  <si>
+    <t>46.346.081/0001-87</t>
+  </si>
+  <si>
+    <t>TesteCNPJ01</t>
+  </si>
+  <si>
+    <t>TesteCNPJ00</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -116,8 +100,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -436,17 +421,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D0D9622-31EC-4FD3-8FA2-68D1F2266F0C}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="17.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="46.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
@@ -461,14 +445,14 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -479,30 +463,11 @@
         <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" t="s">
-        <v>14</v>
-      </c>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C8" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>